<commit_message>
alt pn list updated
alt pn list updated
</commit_message>
<xml_diff>
--- a/mft/pca/BOM/Wilamp DCU ALT MPN (no DNP).xlsx
+++ b/mft/pca/BOM/Wilamp DCU ALT MPN (no DNP).xlsx
@@ -13,16 +13,43 @@
   </bookViews>
   <sheets>
     <sheet name="My Lists Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="bom" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'My Lists Worksheet'!$A$1:$F$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bom!$B$1:$D$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'My Lists Worksheet'!$A$1:$K$85</definedName>
+    <definedName name="Wilamp_DCU_2.0" localSheetId="1">bom!$A$1:$D$85</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Wilamp_DCU 2.0" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\Lorence\Documents\GitHub\Wilamp_DCU\mft\pca\BOM\Wilamp_DCU 2.0.csv" comma="1">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="354">
   <si>
     <t>Index</t>
   </si>
@@ -834,17 +861,273 @@
     <t>MPI4020V2-220-R (different footprint size)</t>
   </si>
   <si>
-    <t>SN74LVC244APWT</t>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>RF Connectors / Coaxial Connectors SMT MALE RECEPT AU</t>
+  </si>
+  <si>
+    <t>IC BUFF/DVR TRI-ST DUAL 20TSSOP</t>
+  </si>
+  <si>
+    <t>Skyworks</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 47K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 43K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 1.5K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 1.2K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Eaton Bussmann</t>
+  </si>
+  <si>
+    <t>MBR0520L</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 0.5A SOD123</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>Inductor RF Chip ThFIXED IND 5.1NH 140MA 700 MOHM</t>
+  </si>
+  <si>
+    <t>FIXED IND 4.3NH 160MA 600 MOHM</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.7NH 220MA 300 MOHM</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors</t>
+  </si>
+  <si>
+    <t>IC RF TXRX+MCU 802.15.4 40-VFQFN</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>CAP CER 10PF 50V 5% NP0 0402</t>
+  </si>
+  <si>
+    <t>CR1220</t>
+  </si>
+  <si>
+    <t>FDK</t>
+  </si>
+  <si>
+    <t>Coin Cell Battery 35mAh 12.5mm</t>
+  </si>
+  <si>
+    <t>BB-2X23</t>
+  </si>
+  <si>
+    <t>Microrobotics</t>
+  </si>
+  <si>
+    <t>Beaglebone 2x23 Pin stacking header(2 Pack )</t>
+  </si>
+  <si>
+    <t>IC CRYPTO 4.5KB I2C</t>
+  </si>
+  <si>
+    <t>Abracon</t>
+  </si>
+  <si>
+    <t>Coin Cell Battery Holders SM COIN CELL B/H</t>
+  </si>
+  <si>
+    <t>74AHC1G32GW,125</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+  </si>
+  <si>
+    <t>IC GATE OR 1CH 2-INP 5TSSOP</t>
+  </si>
+  <si>
+    <t>42-100017-01</t>
+  </si>
+  <si>
+    <t>TSC</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Voltage Regulators - Switching Regulators 42VIN,2A SIMPLE SW NANO STEP-DOWN REG</t>
+  </si>
+  <si>
+    <t>SMBJ40CA</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>TVS DIODE 40VWM 64.5VC DO214AA</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>6-1879336-2</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>Vishay Beyschlag</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0 OHM JUMPER 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0 OHM JUMPER 1/4W 1206</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>MCU 8BIT 32KB FLASH 28SSOP</t>
+  </si>
+  <si>
+    <t>LED RED 0402 SMD</t>
+  </si>
+  <si>
+    <t>LED GREEN 0402 SMD</t>
+  </si>
+  <si>
+    <t>LED CHIPLED 633NM RED 0805 SMD</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>Maxim</t>
+  </si>
+  <si>
+    <t>IC RTC I2C 8SOIC</t>
+  </si>
+  <si>
+    <t>IC INVERTER HS SINGLE SOT-23-5</t>
+  </si>
+  <si>
+    <t>IC INDCT LOAD DRVR AUTO SOT23</t>
+  </si>
+  <si>
+    <t>FERRITE CHIP 120 OHM 0805</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB MINI B R/A SMD</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>CONN RCPT .100" 46POS DUAL GOLD</t>
+  </si>
+  <si>
+    <t>CUI Inc.</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 2.1X5.5MM HIGH CUR</t>
+  </si>
+  <si>
+    <t>Molex, LLC</t>
+  </si>
+  <si>
+    <t>CONN HEADER 7POS .100 VERT TIN</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2POS .100" STR TIN</t>
+  </si>
+  <si>
+    <t>C0603C222K5RACTU</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>CAP CER 2200PF 50V 10% X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805C104K5RACTU</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc.</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>MFT</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Bourns, SMC Diode Solutions</t>
+  </si>
+  <si>
+    <t>TC7SH08FU,LJ(CT</t>
+  </si>
+  <si>
+    <t>please double check</t>
+  </si>
+  <si>
+    <t>SN74LVC244APWT, SN74ALVC244PW</t>
+  </si>
+  <si>
+    <t>in stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -902,17 +1185,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -926,12 +1210,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -944,6 +1246,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wilamp_DCU 2.0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1210,11 +1516,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1222,7 +1528,7 @@
     <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.109375" style="6" customWidth="1"/>
   </cols>
@@ -1240,7 +1546,7 @@
       <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -1264,7 +1570,7 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1272,7 +1578,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1285,7 +1591,7 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1308,7 +1614,7 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1329,7 +1635,7 @@
       <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1350,7 +1656,7 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1371,7 +1677,7 @@
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1392,7 +1698,7 @@
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1400,7 +1706,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1413,7 +1719,7 @@
       <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1436,7 +1742,7 @@
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1444,7 +1750,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1457,7 +1763,7 @@
       <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1480,7 +1786,7 @@
       <c r="D12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1488,7 +1794,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1501,7 +1807,7 @@
       <c r="D13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1524,7 +1830,7 @@
       <c r="D14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1545,7 +1851,7 @@
       <c r="D15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="5" t="s">
         <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1566,7 +1872,7 @@
       <c r="D16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1587,7 +1893,7 @@
       <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1595,7 +1901,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1608,7 +1914,7 @@
       <c r="D18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1631,7 +1937,7 @@
       <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="5" t="s">
         <v>70</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1639,7 +1945,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1652,7 +1958,7 @@
       <c r="D20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="5" t="s">
         <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1675,7 +1981,7 @@
       <c r="D21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1696,7 +2002,7 @@
       <c r="D22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -1704,7 +2010,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1717,7 +2023,7 @@
       <c r="D23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1727,7 +2033,7 @@
         <v>782853131</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1740,7 +2046,7 @@
       <c r="D24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1763,7 +2069,7 @@
       <c r="D25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="5" t="s">
         <v>91</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1771,7 +2077,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" hidden="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1784,7 +2090,7 @@
       <c r="D26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1807,7 +2113,7 @@
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1830,7 +2136,7 @@
       <c r="D28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1851,7 +2157,7 @@
       <c r="D29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="5" t="s">
         <v>104</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1872,7 +2178,7 @@
       <c r="D30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="5" t="s">
         <v>108</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1880,7 +2186,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" hidden="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1893,7 +2199,7 @@
       <c r="D31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1903,7 +2209,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1916,7 +2222,7 @@
       <c r="D32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -1939,7 +2245,7 @@
       <c r="D33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1962,7 +2268,7 @@
       <c r="D34" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -1983,7 +2289,7 @@
       <c r="D35" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="5" t="s">
         <v>122</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -1991,7 +2297,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2004,7 +2310,7 @@
       <c r="D36" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -2027,7 +2333,7 @@
       <c r="D37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="5" t="s">
         <v>129</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -2035,7 +2341,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2048,7 +2354,7 @@
       <c r="D38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -2058,7 +2364,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2071,7 +2377,7 @@
       <c r="D39" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -2094,7 +2400,7 @@
       <c r="D40" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5" t="s">
         <v>137</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -2102,7 +2408,7 @@
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2115,7 +2421,7 @@
       <c r="D41" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -2125,7 +2431,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2138,7 +2444,7 @@
       <c r="D42" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -2161,7 +2467,7 @@
       <c r="D43" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="5" t="s">
         <v>144</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -2182,7 +2488,7 @@
       <c r="D44" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="5" t="s">
         <v>147</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -2203,7 +2509,7 @@
       <c r="D45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="5" t="s">
         <v>150</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -2211,7 +2517,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2224,7 +2530,7 @@
       <c r="D46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -2234,7 +2540,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2247,7 +2553,7 @@
       <c r="D47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F47" s="1" t="s">
@@ -2257,7 +2563,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2270,7 +2576,7 @@
       <c r="D48" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -2280,7 +2586,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2293,7 +2599,7 @@
       <c r="D49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F49" s="1" t="s">
@@ -2303,7 +2609,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2316,7 +2622,7 @@
       <c r="D50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="5" t="s">
         <v>161</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -2324,7 +2630,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2337,7 +2643,7 @@
       <c r="D51" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -2347,7 +2653,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:9" hidden="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2360,7 +2666,7 @@
       <c r="D52" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="5" t="s">
         <v>167</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -2368,28 +2674,28 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>9</v>
+      <c r="B53" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E53" s="15">
+        <v>1025</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2399,10 +2705,10 @@
       <c r="C54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -2412,20 +2718,20 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="B55" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F55" s="1" t="s">
@@ -2433,28 +2739,33 @@
       </c>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="B56" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="H56" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2467,7 +2778,7 @@
       <c r="D57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F57" s="1" t="s">
@@ -2477,7 +2788,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2490,7 +2801,7 @@
       <c r="D58" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="5" t="s">
         <v>177</v>
       </c>
       <c r="F58" s="1" t="s">
@@ -2498,7 +2809,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:9" hidden="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2511,7 +2822,7 @@
       <c r="D59" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="5" t="s">
         <v>180</v>
       </c>
       <c r="F59" s="1" t="s">
@@ -2519,20 +2830,20 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="B60" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="1" t="s">
@@ -2540,28 +2851,28 @@
       </c>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>9</v>
+      <c r="B61" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E61" s="15">
+        <v>41259</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:9" hidden="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2574,7 +2885,7 @@
       <c r="D62" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="5" t="s">
         <v>183</v>
       </c>
       <c r="F62" s="1" t="s">
@@ -2582,7 +2893,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2595,7 +2906,7 @@
       <c r="D63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="5" t="s">
         <v>186</v>
       </c>
       <c r="F63" s="1" t="s">
@@ -2603,7 +2914,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" hidden="1">
+    <row r="64" spans="1:9" hidden="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2616,7 +2927,7 @@
       <c r="D64" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" s="5" t="s">
         <v>189</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -2637,7 +2948,7 @@
       <c r="D65" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="5" t="s">
         <v>192</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -2658,7 +2969,7 @@
       <c r="D66" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="5" t="s">
         <v>195</v>
       </c>
       <c r="F66" s="1" t="s">
@@ -2679,7 +2990,7 @@
       <c r="D67" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" s="5" t="s">
         <v>198</v>
       </c>
       <c r="F67" s="1" t="s">
@@ -2700,7 +3011,7 @@
       <c r="D68" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" s="5" t="s">
         <v>201</v>
       </c>
       <c r="F68" s="1" t="s">
@@ -2721,7 +3032,7 @@
       <c r="D69" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" s="5" t="s">
         <v>204</v>
       </c>
       <c r="F69" s="1" t="s">
@@ -2742,7 +3053,7 @@
       <c r="D70" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="5" t="s">
         <v>207</v>
       </c>
       <c r="F70" s="1" t="s">
@@ -2760,10 +3071,10 @@
       <c r="C71" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F71" s="1" t="s">
@@ -2773,7 +3084,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" hidden="1">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2786,7 +3097,7 @@
       <c r="D72" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="5" t="s">
         <v>213</v>
       </c>
       <c r="F72" s="1" t="s">
@@ -2809,7 +3120,7 @@
       <c r="D73" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" s="5" t="s">
         <v>216</v>
       </c>
       <c r="F73" s="1" t="s">
@@ -2817,7 +3128,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" hidden="1">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2830,7 +3141,7 @@
       <c r="D74" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="5" t="s">
         <v>219</v>
       </c>
       <c r="F74" s="1" t="s">
@@ -2850,10 +3161,10 @@
       <c r="C75" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="1" t="s">
@@ -2863,24 +3174,24 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" hidden="1">
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>9</v>
+      <c r="B76" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="E76" s="15">
+        <v>1240</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="H76" s="5"/>
     </row>
@@ -2897,7 +3208,7 @@
       <c r="D77" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="1" t="s">
@@ -2920,7 +3231,7 @@
       <c r="D78" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" s="5" t="s">
         <v>227</v>
       </c>
       <c r="F78" s="1" t="s">
@@ -2941,7 +3252,7 @@
       <c r="D79" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" s="5" t="s">
         <v>230</v>
       </c>
       <c r="F79" s="1" t="s">
@@ -2962,7 +3273,7 @@
       <c r="D80" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" s="5" t="s">
         <v>233</v>
       </c>
       <c r="F80" s="1" t="s">
@@ -2983,7 +3294,7 @@
       <c r="D81" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" s="5" t="s">
         <v>236</v>
       </c>
       <c r="F81" s="1" t="s">
@@ -3004,7 +3315,7 @@
       <c r="D82" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" s="5" t="s">
         <v>144</v>
       </c>
       <c r="F82" s="1" t="s">
@@ -3025,7 +3336,7 @@
       <c r="D83" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" s="5" t="s">
         <v>240</v>
       </c>
       <c r="F83" s="1" t="s">
@@ -3033,7 +3344,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" hidden="1">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3046,14 +3357,14 @@
       <c r="D84" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H84" s="5" t="s">
-        <v>270</v>
+      <c r="H84" s="4" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:8" hidden="1">
@@ -3069,7 +3380,7 @@
       <c r="D85" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" s="5" t="s">
         <v>245</v>
       </c>
       <c r="F85" s="1" t="s">
@@ -3078,17 +3389,1244 @@
       <c r="H85" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F85">
+  <autoFilter ref="A1:K85">
     <filterColumn colId="5">
       <filters blank="1">
-        <filter val="In Stock - Non-Stock"/>
-        <filter val="In Stock - Value Added"/>
         <filter val="Normally Stocking"/>
         <filter val="Obsolete"/>
-        <filter val="Value Added"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters blank="1">
+        <filter val="cannot FIND ALT MPN"/>
+        <filter val="cannot FIND ALT MPN with same PINOUT"/>
+        <filter val="MPI4020V2-220-R (different footprint size)"/>
+        <filter val="TC7SH08FU,LJ(CT"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E85"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f>IF(ISERROR(VLOOKUP(D4,bom!D27:D85, 1, FALSE)),"Not Exist","Exist" )</f>
+        <v>Not Exist</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="11" t="str">
+        <f>IF(ISERROR(VLOOKUP(D5,bom!D28:D86, 1, FALSE)),"Not Exist","Exist" )</f>
+        <v>Not Exist</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="12">
+        <v>22</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="12">
+        <v>2</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="B15" s="12">
+        <v>5</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="B17" s="12">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" s="12">
+        <v>901200122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18" s="12">
+        <v>2</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D18" s="12">
+        <v>22284070</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="B23" s="12">
+        <v>2</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B25" s="12">
+        <v>5</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="12">
+        <v>3</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B30" s="12">
+        <v>2</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B31" s="12">
+        <v>4</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B32" s="12">
+        <v>2</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B34" s="12">
+        <v>5</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B36" s="12">
+        <v>3</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="12">
+        <v>10</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="12">
+        <v>6</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="12">
+        <v>2</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="12">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="12">
+        <v>1</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="12">
+        <v>3</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="12">
+        <v>9</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="12">
+        <v>1</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="12">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="12">
+        <v>2</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B50" s="12">
+        <v>6</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B52" s="12">
+        <v>3</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B53" s="12">
+        <v>1</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B54" s="12">
+        <v>2</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B55" s="12">
+        <v>2</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B56" s="12">
+        <v>4</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B57" s="12">
+        <v>2</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" s="12">
+        <v>2</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B59" s="12">
+        <v>3</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B61" s="12">
+        <v>2</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" s="12">
+        <v>2</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" s="12">
+        <v>12</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="12">
+        <v>2</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="12">
+        <v>6</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="12">
+        <v>2</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B67" s="12">
+        <v>4</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="12">
+        <v>4</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" s="12">
+        <v>2</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="12">
+        <v>2</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="B71" s="12">
+        <v>2</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B72" s="12">
+        <v>2</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B73" s="12">
+        <v>2</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" s="12">
+        <v>2</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B75" s="12">
+        <v>2</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B76" s="12">
+        <v>2</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" s="12">
+        <v>2</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="12">
+        <v>2</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="B79" s="12">
+        <v>2</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B80" s="12">
+        <v>2</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B81" s="12">
+        <v>2</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B82" s="12">
+        <v>4</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" s="12">
+        <v>2</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B84" s="12">
+        <v>3</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B85" s="12">
+        <v>2</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D85"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NUD3124LT1G labeled as no stock
NUD3124LT1G labeled as no stock
</commit_message>
<xml_diff>
--- a/mft/pca/BOM/Wilamp DCU ALT MPN (no DNP).xlsx
+++ b/mft/pca/BOM/Wilamp DCU ALT MPN (no DNP).xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="357">
   <si>
     <t>Index</t>
   </si>
@@ -1111,16 +1111,32 @@
   </si>
   <si>
     <t>in stock</t>
+  </si>
+  <si>
+    <t>641 In Stock</t>
+  </si>
+  <si>
+    <t>no longer manufactured</t>
+  </si>
+  <si>
+    <t>No Stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1187,16 +1203,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1210,14 +1226,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1226,10 +1242,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1515,12 +1535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1531,6 +1550,7 @@
     <col min="5" max="5" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1578,7 +1598,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1601,7 +1621,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1622,7 +1642,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1643,7 +1663,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1664,7 +1684,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1685,7 +1705,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1706,7 +1726,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1729,7 +1749,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1750,7 +1770,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1773,7 +1793,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1794,7 +1814,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1817,7 +1837,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1838,7 +1858,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1859,7 +1879,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1880,7 +1900,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1901,7 +1921,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1924,7 +1944,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1945,7 +1965,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1968,7 +1988,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1989,7 +2009,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2010,7 +2030,7 @@
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2033,7 +2053,7 @@
         <v>782853131</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2055,8 +2075,14 @@
       <c r="H24" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1">
+      <c r="I24" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2072,12 +2098,14 @@
       <c r="E25" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" hidden="1">
+      <c r="F25" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2100,7 +2128,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2123,7 +2151,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2144,7 +2172,7 @@
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" hidden="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2165,7 +2193,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2186,7 +2214,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" hidden="1">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2209,7 +2237,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2255,7 +2283,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2276,7 +2304,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2297,7 +2325,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2320,7 +2348,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2341,7 +2369,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2364,7 +2392,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2387,7 +2415,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2408,7 +2436,7 @@
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2431,7 +2459,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2454,7 +2482,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2475,7 +2503,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2496,7 +2524,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2517,7 +2545,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2540,7 +2568,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2563,7 +2591,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2586,7 +2614,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2609,7 +2637,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2630,7 +2658,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2653,7 +2681,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2674,7 +2702,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2765,7 +2793,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2788,7 +2816,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2809,7 +2837,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2872,7 +2900,7 @@
       </c>
       <c r="H61" s="5"/>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2893,7 +2921,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2914,7 +2942,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2935,7 +2963,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" hidden="1">
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2956,7 +2984,7 @@
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" hidden="1">
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2977,7 +3005,7 @@
       </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" hidden="1">
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2998,7 +3026,7 @@
       </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" hidden="1">
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3019,7 +3047,7 @@
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" hidden="1">
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3040,7 +3068,7 @@
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" hidden="1">
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3084,7 +3112,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1">
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3107,7 +3135,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1">
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3128,7 +3156,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" hidden="1">
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3174,7 +3202,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1">
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3218,7 +3246,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1">
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3239,7 +3267,7 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" hidden="1">
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3260,7 +3288,7 @@
       </c>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" hidden="1">
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3281,7 +3309,7 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" hidden="1">
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3302,7 +3330,7 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" hidden="1">
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3323,7 +3351,7 @@
       </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" hidden="1">
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3344,7 +3372,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" hidden="1">
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3367,7 +3395,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1">
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3389,22 +3417,7 @@
       <c r="H85" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K85">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="Normally Stocking"/>
-        <filter val="Obsolete"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters blank="1">
-        <filter val="cannot FIND ALT MPN"/>
-        <filter val="cannot FIND ALT MPN with same PINOUT"/>
-        <filter val="MPI4020V2-220-R (different footprint size)"/>
-        <filter val="TC7SH08FU,LJ(CT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K85"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3414,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3795,7 +3808,7 @@
       <c r="C26" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="18" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>